<commit_message>
small updates on data tables
</commit_message>
<xml_diff>
--- a/Cabana_app/MyCabin_database_structure.xlsx
+++ b/Cabana_app/MyCabin_database_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CabinApp\Cabana_app\Cabana_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAAEAFE-6A8E-46C9-986C-EC53CB9F1A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E542B7EA-CF06-41AE-ACDD-C8FF4604A148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8595" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{AE9CDD31-9878-4641-8DDA-F2D5F6DA53FE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="130">
   <si>
     <t>Tudor</t>
   </si>
@@ -450,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -922,7 +928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -986,6 +992,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1004,15 +1106,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1031,123 +1127,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1173,64 +1189,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C50D95-9DC3-F487-834F-FAA638B78B40}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="628650" y="276225"/>
-          <a:ext cx="9077325" cy="123825"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1402,14 +1360,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1158240</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>481965</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -1426,8 +1384,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1158240" y="2152650"/>
-          <a:ext cx="6204585" cy="1314450"/>
+          <a:off x="2914650" y="304800"/>
+          <a:ext cx="5053965" cy="3171825"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1779,7 +1737,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,18 +1765,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
       <c r="K1" s="1"/>
       <c r="M1" t="s">
         <v>79</v>
@@ -1875,28 +1833,29 @@
     </row>
     <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
-      <c r="K5" s="38" t="s">
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="40"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="70"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -1921,9 +1880,12 @@
         <v>2</v>
       </c>
       <c r="H6" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="J6" s="28" t="s">
         <v>49</v>
       </c>
       <c r="K6" s="11" t="s">
@@ -1980,9 +1942,12 @@
         <v>3</v>
       </c>
       <c r="H7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="17" t="s">
@@ -2069,16 +2034,16 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="66"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
       <c r="K10" s="14">
         <v>3</v>
       </c>
@@ -2120,13 +2085,13 @@
       <c r="E11" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="14">
         <v>4</v>
       </c>
@@ -2165,10 +2130,10 @@
       <c r="E12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
       <c r="K12" s="14">
         <v>5</v>
       </c>
@@ -2195,10 +2160,10 @@
       <c r="A13" s="1"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
       <c r="K13" s="14">
         <v>6</v>
       </c>
@@ -2225,10 +2190,10 @@
       <c r="A14" s="1"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
       <c r="K14" s="14">
         <v>7</v>
       </c>
@@ -2252,18 +2217,18 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
       <c r="K15" s="14">
         <v>8</v>
       </c>
@@ -2416,20 +2381,20 @@
     </row>
     <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="43"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="73"/>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2592,17 +2557,17 @@
     </row>
     <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
@@ -2664,13 +2629,13 @@
     </row>
     <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
@@ -2710,14 +2675,14 @@
       <c r="N47" s="2"/>
     </row>
     <row r="52" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G52" s="44" t="s">
+      <c r="G52" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="44"/>
-      <c r="L52" s="44" t="s">
+      <c r="H52" s="57"/>
+      <c r="L52" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="M52" s="44"/>
+      <c r="M52" s="57"/>
     </row>
     <row r="53" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G53" t="s">
@@ -2790,16 +2755,15 @@
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="G52:H52"/>
     <mergeCell ref="L52:M52"/>
-    <mergeCell ref="A5:I5"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="K5:S5"/>
     <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2808,7 +2772,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2820,9 +2784,9 @@
     <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
@@ -2831,805 +2795,793 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="60"/>
-    </row>
-    <row r="2" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="76"/>
+    </row>
+    <row r="2" spans="1:26" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-    </row>
-    <row r="3" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54">
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+    </row>
+    <row r="3" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="34">
         <v>1</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="45">
         <v>45344</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="34">
         <v>2</v>
       </c>
-      <c r="F3" s="72">
+      <c r="F3" s="45">
         <v>45350</v>
       </c>
-      <c r="G3" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-    </row>
-    <row r="4" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54">
+      <c r="G3" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="34"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+    </row>
+    <row r="4" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34">
         <v>2</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="34">
         <v>1</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="45">
         <v>45344</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="34">
         <v>2</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="45">
         <v>45350</v>
       </c>
-      <c r="G4" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="52"/>
-    </row>
-    <row r="5" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54">
-        <v>3</v>
-      </c>
-      <c r="B5" s="56" t="s">
+      <c r="G4" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="34"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+    </row>
+    <row r="5" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34">
+        <v>3</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="34">
         <v>1</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="45">
         <v>45344</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="34">
         <v>2</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5" s="45">
         <v>45350</v>
       </c>
-      <c r="G5" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="54"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="52"/>
-      <c r="Z5" s="52"/>
-    </row>
-    <row r="6" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54">
+      <c r="G5" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+    </row>
+    <row r="6" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34">
         <v>4</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="45">
         <v>45344</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="34">
         <v>2</v>
       </c>
-      <c r="F6" s="72">
+      <c r="F6" s="45">
         <v>45350</v>
       </c>
-      <c r="G6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="54"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="52"/>
-      <c r="Z6" s="52"/>
-    </row>
-    <row r="7" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="54">
+      <c r="G6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="34"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+    </row>
+    <row r="7" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34">
         <v>5</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="34">
         <v>1</v>
       </c>
-      <c r="D7" s="72">
+      <c r="D7" s="45">
         <v>45344</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="34">
         <v>2</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7" s="45">
         <v>45350</v>
       </c>
-      <c r="G7" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" s="54"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
+      <c r="G7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="34"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
     </row>
     <row r="9" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="76"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="67" t="s">
+      <c r="G11" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="34">
         <v>1</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="34">
         <v>2</v>
       </c>
-      <c r="E12" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
+      <c r="E12" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="78">
+      <c r="A13" s="49">
         <v>2</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="49"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="50"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="78">
-        <v>3</v>
-      </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="49"/>
+      <c r="A14" s="49">
+        <v>3</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="50"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="78">
+      <c r="A15" s="49">
         <v>4</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="49"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="61">
+      <c r="A16" s="37">
         <v>5</v>
       </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="49"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H17" s="49"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="49"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="48"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="66" t="s">
+      <c r="E20" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="66" t="s">
+      <c r="F20" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="H20" s="66" t="s">
+      <c r="H20" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="I20" s="66" t="s">
+      <c r="I20" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="J20" s="66" t="s">
+      <c r="J20" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="K20" s="67" t="s">
+      <c r="K20" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="56" t="s">
+      <c r="D21" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="54" t="b">
+      <c r="G21" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="H21" s="72" t="b">
+      <c r="H21" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="81"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="81"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="81"/>
+      <c r="I21" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="52"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="52"/>
     </row>
     <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="80" t="s">
+      <c r="D22" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="86" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="62" t="b">
+      <c r="G22" s="38" t="b">
         <v>0</v>
       </c>
-      <c r="H22" s="82" t="b">
+      <c r="H22" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="82" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="L22" s="81"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="81"/>
+      <c r="I22" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="L22" s="52"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="52"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="74"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="74"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="74"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="70"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="83"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="66" t="s">
+      <c r="E29" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="66" t="s">
+      <c r="F29" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="66" t="s">
+      <c r="G29" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="H29" s="66" t="s">
+      <c r="H29" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="I29" s="67" t="s">
+      <c r="J29" s="43" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="71" t="s">
+      <c r="A30" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="H30" s="62" t="s">
+      <c r="D30" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I30" s="63" t="s">
+      <c r="J30" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="O31" s="57" t="s">
+      <c r="O31" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="P31" s="57" t="s">
+      <c r="P31" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="Q31" s="57" t="s">
+      <c r="Q31" s="36" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="34" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="F34" s="55" t="s">
+      <c r="F34" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55" t="s">
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="55"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="55"/>
-      <c r="T34" s="55"/>
-      <c r="U34" s="55"/>
-      <c r="V34" s="55"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
+      <c r="P34" s="77"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="77"/>
+      <c r="S34" s="77"/>
+      <c r="T34" s="77"/>
+      <c r="U34" s="77"/>
+      <c r="V34" s="77"/>
     </row>
     <row r="35" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55" t="s">
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="55"/>
-      <c r="U35" s="55"/>
-      <c r="V35" s="55"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="77"/>
+      <c r="L35" s="77"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="77"/>
+      <c r="P35" s="77"/>
+      <c r="Q35" s="77"/>
+      <c r="R35" s="77"/>
+      <c r="S35" s="77"/>
+      <c r="T35" s="77"/>
+      <c r="U35" s="77"/>
+      <c r="V35" s="77"/>
     </row>
     <row r="36" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="F36" s="55" t="s">
+      <c r="F36" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55" t="s">
+      <c r="G36" s="77"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="55"/>
-      <c r="T36" s="55"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="55"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="77"/>
+      <c r="L36" s="77"/>
+      <c r="M36" s="77"/>
+      <c r="N36" s="77"/>
+      <c r="O36" s="77"/>
+      <c r="P36" s="77"/>
+      <c r="Q36" s="77"/>
+      <c r="R36" s="77"/>
+      <c r="S36" s="77"/>
+      <c r="T36" s="77"/>
+      <c r="U36" s="77"/>
+      <c r="V36" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3637,12 +3589,12 @@
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="I36:V36"/>
     <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A28:I28"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="I34:V34"/>
     <mergeCell ref="I35:V35"/>
+    <mergeCell ref="A28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Logo images & some business documents created
</commit_message>
<xml_diff>
--- a/Cabana_app/MyCabin_database_structure.xlsx
+++ b/Cabana_app/MyCabin_database_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CabinApp\Cabana_app\Cabana_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E542B7EA-CF06-41AE-ACDD-C8FF4604A148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1236E686-310D-444B-8F20-59400D8F4640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8595" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{AE9CDD31-9878-4641-8DDA-F2D5F6DA53FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AE9CDD31-9878-4641-8DDA-F2D5F6DA53FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="131">
   <si>
     <t>Tudor</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>auth.uid()</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -928,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1037,9 +1040,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1070,6 +1070,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1079,15 +1088,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1127,6 +1127,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1155,15 +1164,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1192,16 +1192,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>973455</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>891540</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1216,8 +1216,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2316480" y="2524125"/>
-          <a:ext cx="7620" cy="2649855"/>
+          <a:off x="891540" y="2247900"/>
+          <a:ext cx="1051560" cy="3034665"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1248,16 +1248,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1539240</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>963930</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1271,9 +1271,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="2882265" y="3754755"/>
-          <a:ext cx="775335" cy="693420"/>
+        <a:xfrm flipV="1">
+          <a:off x="963930" y="4010025"/>
+          <a:ext cx="941070" cy="1377315"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1765,18 +1765,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="58"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
       <c r="K1" s="1"/>
       <c r="M1" t="s">
         <v>79</v>
@@ -1833,29 +1833,29 @@
     </row>
     <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="68" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="70"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="69"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -2034,12 +2034,12 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
@@ -2217,14 +2217,14 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
@@ -2381,20 +2381,20 @@
     </row>
     <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="73"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="72"/>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2557,17 +2557,17 @@
     </row>
     <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="56"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
@@ -2629,13 +2629,13 @@
     </row>
     <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="63"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="62"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
@@ -2675,14 +2675,14 @@
       <c r="N47" s="2"/>
     </row>
     <row r="52" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G52" s="57" t="s">
+      <c r="G52" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="57"/>
-      <c r="L52" s="57" t="s">
+      <c r="H52" s="59"/>
+      <c r="L52" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="M52" s="57"/>
+      <c r="M52" s="59"/>
     </row>
     <row r="53" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G53" t="s">
@@ -2772,7 +2772,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2795,29 +2795,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="78"/>
     </row>
     <row r="2" spans="1:26" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
@@ -2881,38 +2881,38 @@
       <c r="C3" s="34">
         <v>1</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="44">
         <v>45344</v>
       </c>
       <c r="E3" s="34">
         <v>2</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="44">
         <v>45350</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="44" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="44" t="s">
         <v>45</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="44" t="s">
         <v>45</v>
       </c>
       <c r="M3" s="34"/>
-      <c r="N3" s="45"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="32"/>
       <c r="P3" s="34"/>
-      <c r="Q3" s="45"/>
+      <c r="Q3" s="44"/>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
       <c r="T3" s="32"/>
@@ -2933,38 +2933,38 @@
       <c r="C4" s="34">
         <v>1</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="44">
         <v>45344</v>
       </c>
       <c r="E4" s="34">
         <v>2</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="44">
         <v>45350</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="44" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="44" t="s">
         <v>45</v>
       </c>
       <c r="K4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="44" t="s">
         <v>45</v>
       </c>
       <c r="M4" s="34"/>
-      <c r="N4" s="45"/>
+      <c r="N4" s="44"/>
       <c r="O4" s="32"/>
       <c r="P4" s="34"/>
-      <c r="Q4" s="45"/>
+      <c r="Q4" s="44"/>
       <c r="R4" s="32"/>
       <c r="S4" s="32"/>
       <c r="T4" s="32"/>
@@ -2985,38 +2985,38 @@
       <c r="C5" s="34">
         <v>1</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <v>45344</v>
       </c>
       <c r="E5" s="34">
         <v>2</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <v>45350</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="44" t="s">
         <v>45</v>
       </c>
       <c r="I5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="44" t="s">
         <v>45</v>
       </c>
       <c r="K5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="44" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="34"/>
-      <c r="N5" s="45"/>
+      <c r="N5" s="44"/>
       <c r="O5" s="32"/>
       <c r="P5" s="34"/>
-      <c r="Q5" s="45"/>
+      <c r="Q5" s="44"/>
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
       <c r="T5" s="32"/>
@@ -3037,38 +3037,38 @@
       <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <v>45344</v>
       </c>
       <c r="E6" s="34">
         <v>2</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="44">
         <v>45350</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="44" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="44" t="s">
         <v>45</v>
       </c>
       <c r="K6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="45" t="s">
+      <c r="L6" s="44" t="s">
         <v>45</v>
       </c>
       <c r="M6" s="34"/>
-      <c r="N6" s="45"/>
+      <c r="N6" s="44"/>
       <c r="O6" s="32"/>
       <c r="P6" s="34"/>
-      <c r="Q6" s="45"/>
+      <c r="Q6" s="44"/>
       <c r="R6" s="32"/>
       <c r="S6" s="32"/>
       <c r="T6" s="32"/>
@@ -3089,38 +3089,38 @@
       <c r="C7" s="34">
         <v>1</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
         <v>45344</v>
       </c>
       <c r="E7" s="34">
         <v>2</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <v>45350</v>
       </c>
       <c r="G7" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="44" t="s">
         <v>45</v>
       </c>
       <c r="I7" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="44" t="s">
         <v>45</v>
       </c>
       <c r="K7" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="45" t="s">
+      <c r="L7" s="44" t="s">
         <v>45</v>
       </c>
       <c r="M7" s="34"/>
-      <c r="N7" s="45"/>
+      <c r="N7" s="44"/>
       <c r="O7" s="32"/>
       <c r="P7" s="34"/>
-      <c r="Q7" s="45"/>
+      <c r="Q7" s="44"/>
       <c r="R7" s="32"/>
       <c r="S7" s="32"/>
       <c r="T7" s="32"/>
@@ -3133,15 +3133,15 @@
     </row>
     <row r="9" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="76"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
@@ -3167,7 +3167,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="53" t="s">
         <v>101</v>
       </c>
       <c r="B12" s="40" t="s">
@@ -3185,12 +3185,12 @@
       <c r="F12" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="49" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="49">
+      <c r="A13" s="48">
         <v>2</v>
       </c>
       <c r="B13" s="34"/>
@@ -3198,13 +3198,13 @@
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
-      <c r="G13" s="50"/>
+      <c r="G13" s="49"/>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
       <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="49">
+      <c r="A14" s="48">
         <v>3</v>
       </c>
       <c r="B14" s="34"/>
@@ -3212,13 +3212,13 @@
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
-      <c r="G14" s="50"/>
+      <c r="G14" s="49"/>
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="49">
+      <c r="A15" s="48">
         <v>4</v>
       </c>
       <c r="B15" s="34"/>
@@ -3226,7 +3226,7 @@
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
-      <c r="G15" s="50"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -3253,24 +3253,24 @@
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="41" t="s">
@@ -3283,9 +3283,9 @@
         <v>18</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="84" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="54" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="42" t="s">
@@ -3313,19 +3313,19 @@
       <c r="P20" s="31"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>114</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="55" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="35" t="s">
@@ -3334,29 +3334,29 @@
       <c r="G21" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="H21" s="45" t="b">
+      <c r="H21" s="44" t="b">
         <v>1</v>
       </c>
       <c r="I21" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="52"/>
+      <c r="J21" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="51"/>
       <c r="M21" s="29"/>
-      <c r="N21" s="52"/>
+      <c r="N21" s="51"/>
       <c r="O21" s="29"/>
-      <c r="P21" s="52"/>
+      <c r="P21" s="51"/>
     </row>
     <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="45" t="s">
         <v>114</v>
       </c>
       <c r="C22" s="38" t="s">
@@ -3365,32 +3365,32 @@
       <c r="D22" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="86" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="51" t="s">
+      <c r="E22" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="50" t="s">
         <v>101</v>
       </c>
       <c r="G22" s="38" t="b">
         <v>0</v>
       </c>
-      <c r="H22" s="53" t="b">
+      <c r="H22" s="52" t="b">
         <v>1</v>
       </c>
       <c r="I22" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="53" t="s">
+      <c r="J22" s="52" t="s">
         <v>45</v>
       </c>
       <c r="K22" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="L22" s="52"/>
+      <c r="L22" s="51"/>
       <c r="M22" s="29"/>
-      <c r="N22" s="52"/>
+      <c r="N22" s="51"/>
       <c r="O22" s="29"/>
-      <c r="P22" s="52"/>
+      <c r="P22" s="51"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="29"/>
@@ -3426,42 +3426,42 @@
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="82"/>
-      <c r="J28" s="83"/>
+      <c r="A28" s="83" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="85"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="42" t="s">
+      <c r="F29" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="42" t="s">
+      <c r="G29" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H29" s="84" t="s">
+      <c r="H29" s="54" t="s">
         <v>6</v>
       </c>
       <c r="I29" s="42" t="s">
@@ -3475,25 +3475,25 @@
       <c r="A30" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="H30" s="86" t="s">
+      <c r="D30" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="56" t="s">
         <v>3</v>
       </c>
       <c r="I30" s="38" t="s">
@@ -3515,73 +3515,73 @@
       </c>
     </row>
     <row r="34" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="F34" s="77" t="s">
+      <c r="F34" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77" t="s">
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="77"/>
-      <c r="R34" s="77"/>
-      <c r="S34" s="77"/>
-      <c r="T34" s="77"/>
-      <c r="U34" s="77"/>
-      <c r="V34" s="77"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="79"/>
+      <c r="P34" s="79"/>
+      <c r="Q34" s="79"/>
+      <c r="R34" s="79"/>
+      <c r="S34" s="79"/>
+      <c r="T34" s="79"/>
+      <c r="U34" s="79"/>
+      <c r="V34" s="79"/>
     </row>
     <row r="35" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="F35" s="77" t="s">
+      <c r="F35" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77" t="s">
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="J35" s="77"/>
-      <c r="K35" s="77"/>
-      <c r="L35" s="77"/>
-      <c r="M35" s="77"/>
-      <c r="N35" s="77"/>
-      <c r="O35" s="77"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="77"/>
-      <c r="R35" s="77"/>
-      <c r="S35" s="77"/>
-      <c r="T35" s="77"/>
-      <c r="U35" s="77"/>
-      <c r="V35" s="77"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="79"/>
+      <c r="T35" s="79"/>
+      <c r="U35" s="79"/>
+      <c r="V35" s="79"/>
     </row>
     <row r="36" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="F36" s="77" t="s">
+      <c r="F36" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77" t="s">
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="J36" s="77"/>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
-      <c r="M36" s="77"/>
-      <c r="N36" s="77"/>
-      <c r="O36" s="77"/>
-      <c r="P36" s="77"/>
-      <c r="Q36" s="77"/>
-      <c r="R36" s="77"/>
-      <c r="S36" s="77"/>
-      <c r="T36" s="77"/>
-      <c r="U36" s="77"/>
-      <c r="V36" s="77"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="79"/>
+      <c r="O36" s="79"/>
+      <c r="P36" s="79"/>
+      <c r="Q36" s="79"/>
+      <c r="R36" s="79"/>
+      <c r="S36" s="79"/>
+      <c r="T36" s="79"/>
+      <c r="U36" s="79"/>
+      <c r="V36" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>